<commit_message>
Preliminary 1Q23 Earnings Release
</commit_message>
<xml_diff>
--- a/ASRT Model.xlsx
+++ b/ASRT Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evan/Documents/GitHub/ASTR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73CDFF5-24AA-C14A-9C64-6B9A1CCB62B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE82C48-B784-EF48-8E84-C7E0F94087B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{A0DF5598-9F1E-6445-A0B8-833A8CBF5F59}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,6 +505,13 @@
       <i/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -530,12 +537,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,10 +880,10 @@
   <dimension ref="A2:AH139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomRight" activeCell="R94" sqref="R94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1077,14 +1085,18 @@
       <c r="L7">
         <v>14541</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>21357</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <v>22841</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="5">
         <v>21869</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>AC7-P7-O7-N7</f>
+        <v>34271</v>
       </c>
       <c r="AA7">
         <v>31684</v>
@@ -1100,14 +1112,18 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <v>3078</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="5">
         <v>2616</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="5">
         <v>3004</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" ref="Q8:Q13" si="2">AC8-P8-O8-N8</f>
+        <v>2450</v>
       </c>
       <c r="AC8">
         <v>11148</v>
@@ -1117,6 +1133,10 @@
       <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="Q9" s="5">
+        <f>AC9-P9-O9-N9</f>
+        <v>1768</v>
+      </c>
       <c r="AC9">
         <v>1768</v>
       </c>
@@ -1137,14 +1157,18 @@
       <c r="L10">
         <v>2272</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <v>1766</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="5">
         <v>2216</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="5">
         <v>2455</v>
+      </c>
+      <c r="Q10" s="5">
+        <f t="shared" si="2"/>
+        <v>2673</v>
       </c>
       <c r="AA10">
         <v>11077</v>
@@ -1183,14 +1207,18 @@
       <c r="L11">
         <v>5038</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <v>5473</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="5">
         <v>6183</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="5">
         <v>5808</v>
+      </c>
+      <c r="Q11" s="5">
+        <f t="shared" si="2"/>
+        <v>7256</v>
       </c>
       <c r="Z11">
         <v>32453</v>
@@ -1232,14 +1260,18 @@
       <c r="L12">
         <v>1999</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="5">
         <v>2228</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="5">
         <v>216</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="5">
         <v>259</v>
+      </c>
+      <c r="Q12" s="5">
+        <f t="shared" si="2"/>
+        <v>661</v>
       </c>
       <c r="Z12">
         <v>12498</v>
@@ -1283,14 +1315,18 @@
       <c r="L13">
         <v>2147</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <v>1644</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="5">
         <v>1358</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="5">
         <v>884</v>
+      </c>
+      <c r="Q13" s="5">
+        <f t="shared" si="2"/>
+        <v>787</v>
       </c>
       <c r="Z13">
         <v>63855</v>
@@ -1349,6 +1385,13 @@
         <f>P7+P8+P9+P10+P11+P12+P13</f>
         <v>34279</v>
       </c>
+      <c r="Q14">
+        <f>Q7+Q8+Q9+Q10+Q11+Q12+Q13</f>
+        <v>49866</v>
+      </c>
+      <c r="R14" s="5">
+        <v>41769</v>
+      </c>
       <c r="Z14">
         <f>Z7+Z8+Z9+Z10+Z11+Z12+Z13</f>
         <v>108806</v>
@@ -1393,14 +1436,18 @@
       <c r="L16">
         <v>416</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="5">
         <v>992</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="5">
         <v>451</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="5">
         <v>473</v>
+      </c>
+      <c r="Q16" s="5">
+        <f t="shared" ref="Q16:Q17" si="3">AC16-P16-O16-N16</f>
+        <v>487</v>
       </c>
       <c r="Z16">
         <v>2084</v>
@@ -1435,11 +1482,16 @@
       <c r="L17">
         <v>-941</v>
       </c>
-      <c r="O17">
+      <c r="N17" s="5"/>
+      <c r="O17" s="5">
         <v>-750</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="5">
         <v>-540</v>
+      </c>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5">
+        <v>697</v>
       </c>
       <c r="Z17">
         <v>118614</v>
@@ -1463,23 +1515,23 @@
         <v>57929</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:G18" si="2">C17+C16+C14</f>
+        <f t="shared" ref="C18:G18" si="4">C17+C16+C14</f>
         <v>57203</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9659</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20617</v>
       </c>
       <c r="J18">
@@ -1506,6 +1558,14 @@
         <f>P14+P17+P16</f>
         <v>34212</v>
       </c>
+      <c r="Q18">
+        <f>Q14+Q17+Q16</f>
+        <v>50353</v>
+      </c>
+      <c r="R18">
+        <f>R14+R17+R16</f>
+        <v>42466</v>
+      </c>
       <c r="Z18">
         <f>Z14+Z17+Z16</f>
         <v>229504</v>
@@ -1561,6 +1621,14 @@
         <f>P14</f>
         <v>34279</v>
       </c>
+      <c r="Q22">
+        <f>Q14</f>
+        <v>49866</v>
+      </c>
+      <c r="R22">
+        <f>R14</f>
+        <v>41769</v>
+      </c>
       <c r="Z22">
         <f>Z14</f>
         <v>108806</v>
@@ -1583,43 +1651,51 @@
         <v>16</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:K24" si="3">J16</f>
+        <f t="shared" ref="J23:K24" si="5">J16</f>
         <v>434</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>542</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L23" si="4">L16</f>
+        <f t="shared" ref="L23" si="6">L16</f>
         <v>416</v>
       </c>
       <c r="N23">
-        <f t="shared" ref="N23:O23" si="5">N16</f>
+        <f t="shared" ref="N23:O23" si="7">N16</f>
         <v>992</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>451</v>
       </c>
       <c r="P23">
-        <f t="shared" ref="P23" si="6">P16</f>
+        <f t="shared" ref="P23:Q23" si="8">P16</f>
         <v>473</v>
       </c>
+      <c r="Q23">
+        <f t="shared" ref="Q23:R23" si="9">Q16</f>
+        <v>487</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="Z23">
-        <f t="shared" ref="Z23:AC24" si="7">Z16</f>
+        <f t="shared" ref="Z23:AC24" si="10">Z16</f>
         <v>2084</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1519</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2579</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2403</v>
       </c>
     </row>
@@ -1628,39 +1704,43 @@
         <v>10</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>378</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-413</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:P24" si="8">L17</f>
+        <f t="shared" ref="L24:Q24" si="11">L17</f>
         <v>-941</v>
       </c>
       <c r="O24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-750</v>
       </c>
       <c r="P24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-540</v>
       </c>
+      <c r="R24">
+        <f>R17</f>
+        <v>697</v>
+      </c>
       <c r="Z24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>118614</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>11258</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-985</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1290</v>
       </c>
     </row>
@@ -1692,6 +1772,14 @@
         <f>P24+P23+P22</f>
         <v>34212</v>
       </c>
+      <c r="Q25">
+        <f>Q24+Q23+Q22</f>
+        <v>50353</v>
+      </c>
+      <c r="R25">
+        <f>R24+R23+R22</f>
+        <v>42466</v>
+      </c>
       <c r="Z25">
         <f>Z24+Z23+Z22</f>
         <v>229504</v>
@@ -1725,6 +1813,9 @@
       <c r="O27">
         <v>4528</v>
       </c>
+      <c r="R27" s="5">
+        <v>5467</v>
+      </c>
       <c r="Z27">
         <v>9505</v>
       </c>
@@ -1747,11 +1838,11 @@
         <v>22873</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:L28" si="9">K25-K27</f>
+        <f t="shared" ref="K28:L28" si="12">K25-K27</f>
         <v>21452</v>
       </c>
       <c r="L28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25472</v>
       </c>
       <c r="N28">
@@ -1759,12 +1850,16 @@
         <v>32343</v>
       </c>
       <c r="O28">
-        <f t="shared" ref="O28:P28" si="10">O25-O27</f>
+        <f t="shared" ref="O28:Q28" si="13">O25-O27</f>
         <v>30603</v>
       </c>
       <c r="P28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>34212</v>
+      </c>
+      <c r="R28">
+        <f>R25-R27</f>
+        <v>36999</v>
       </c>
       <c r="Z28">
         <f>Z25-Z27</f>
@@ -1810,6 +1905,9 @@
       <c r="O30">
         <v>10543</v>
       </c>
+      <c r="R30" s="5">
+        <v>16904</v>
+      </c>
       <c r="Z30">
         <v>108866</v>
       </c>
@@ -1850,6 +1948,9 @@
       <c r="O32">
         <v>1300</v>
       </c>
+      <c r="R32" s="5">
+        <v>9167</v>
+      </c>
       <c r="AB32">
         <v>3914</v>
       </c>
@@ -1873,6 +1974,9 @@
       <c r="O33">
         <v>7969</v>
       </c>
+      <c r="R33" s="5">
+        <v>6284</v>
+      </c>
       <c r="Z33">
         <v>101774</v>
       </c>
@@ -1912,11 +2016,11 @@
         <v>7507</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:L35" si="11">K28-K30-K32-K33-K34-K31-K29</f>
+        <f t="shared" ref="K35:L35" si="14">K28-K30-K32-K33-K34-K31-K29</f>
         <v>-12001</v>
       </c>
       <c r="L35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>25472</v>
       </c>
       <c r="N35">
@@ -1931,6 +2035,10 @@
         <f>P28-P30-P32-P33-P34-P31-P29</f>
         <v>34212</v>
       </c>
+      <c r="R35">
+        <f>R28-R30-R32-R33-R34-R31-R29</f>
+        <v>4644</v>
+      </c>
       <c r="Z35">
         <f>Z28-Z30-Z32-Z33-Z34-Z31-Z29</f>
         <v>-194428</v>
@@ -1940,11 +2048,11 @@
         <v>-82155</v>
       </c>
       <c r="AB35">
-        <f t="shared" ref="AB35:AC35" si="12">AB28-AB30-AB32-AB33-AB34-AB31-AB29</f>
+        <f t="shared" ref="AB35:AC35" si="15">AB28-AB30-AB32-AB33-AB34-AB31-AB29</f>
         <v>9424</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>39405</v>
       </c>
     </row>
@@ -1996,6 +2104,9 @@
       <c r="O41">
         <v>-2269</v>
       </c>
+      <c r="R41" s="5">
+        <v>-1122</v>
+      </c>
       <c r="Z41">
         <v>-58389</v>
       </c>
@@ -2025,6 +2136,10 @@
       <c r="O42">
         <v>-95</v>
       </c>
+      <c r="R42" s="5">
+        <f>802+-9918</f>
+        <v>-9116</v>
+      </c>
       <c r="Z42">
         <v>3948</v>
       </c>
@@ -2047,11 +2162,11 @@
         <v>-2415</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43:L43" si="13">K42+K41</f>
+        <f t="shared" ref="K43:L43" si="16">K42+K41</f>
         <v>-2468</v>
       </c>
       <c r="L43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N43">
@@ -2059,12 +2174,16 @@
         <v>-1782</v>
       </c>
       <c r="O43">
-        <f t="shared" ref="O43:P43" si="14">O42+O41</f>
+        <f t="shared" ref="O43:R43" si="17">O42+O41</f>
         <v>-2364</v>
       </c>
       <c r="P43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="17"/>
+        <v>-10238</v>
       </c>
       <c r="Z43">
         <f>Z42+Z41</f>
@@ -2092,11 +2211,11 @@
         <v>5092</v>
       </c>
       <c r="K44">
-        <f t="shared" ref="K44:L44" si="15">K35+K43</f>
+        <f t="shared" ref="K44:L44" si="18">K35+K43</f>
         <v>-14469</v>
       </c>
       <c r="L44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>25472</v>
       </c>
       <c r="N44">
@@ -2104,12 +2223,20 @@
         <v>9777</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44:P44" si="16">O35+O43</f>
+        <f t="shared" ref="O44:R44" si="19">O35+O43</f>
         <v>8427</v>
       </c>
       <c r="P44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>34212</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="19"/>
+        <v>-5594</v>
       </c>
       <c r="Z44">
         <f>Z35+Z43</f>
@@ -2141,6 +2268,9 @@
       <c r="N46">
         <v>-713</v>
       </c>
+      <c r="R46" s="5">
+        <v>2110</v>
+      </c>
       <c r="Z46">
         <v>5283</v>
       </c>
@@ -2166,6 +2296,10 @@
         <f>N44+N46</f>
         <v>9064</v>
       </c>
+      <c r="R47">
+        <f>R44+R46</f>
+        <v>-3484</v>
+      </c>
       <c r="Z47">
         <f>Z44+Z46</f>
         <v>-243586</v>
@@ -2195,6 +2329,10 @@
         <f>N47/N51</f>
         <v>0.23963620981387479</v>
       </c>
+      <c r="R49" s="2">
+        <f>R47/R51</f>
+        <v>-6.8307028722674246E-2</v>
+      </c>
       <c r="Z49" s="2">
         <f>Z47/Z51</f>
         <v>-3.4445670003959501</v>
@@ -2224,6 +2362,10 @@
         <f>N47/N52</f>
         <v>0.23555093555093556</v>
       </c>
+      <c r="R50" s="2">
+        <f>R47/R52</f>
+        <v>-6.8307028722674246E-2</v>
+      </c>
       <c r="Z50" s="2">
         <f>Z47/Z52</f>
         <v>-3.4445670003959501</v>
@@ -2251,6 +2393,9 @@
       <c r="N51">
         <v>37824</v>
       </c>
+      <c r="R51">
+        <v>51005</v>
+      </c>
       <c r="Z51">
         <v>70716</v>
       </c>
@@ -2274,6 +2419,9 @@
       <c r="N52">
         <v>38480</v>
       </c>
+      <c r="R52">
+        <v>51005</v>
+      </c>
       <c r="Z52">
         <v>70716</v>
       </c>
@@ -2307,6 +2455,9 @@
       <c r="N59">
         <v>61389</v>
       </c>
+      <c r="R59">
+        <v>68603</v>
+      </c>
       <c r="AB59">
         <v>36810</v>
       </c>
@@ -2324,6 +2475,9 @@
       <c r="N60">
         <v>48923</v>
       </c>
+      <c r="R60">
+        <v>46466</v>
+      </c>
       <c r="AB60">
         <v>44361</v>
       </c>
@@ -2341,6 +2495,9 @@
       <c r="N61">
         <v>9480</v>
       </c>
+      <c r="R61">
+        <v>16226</v>
+      </c>
       <c r="AB61">
         <v>7489</v>
       </c>
@@ -2358,6 +2515,9 @@
       <c r="N62">
         <v>5323</v>
       </c>
+      <c r="R62">
+        <v>6554</v>
+      </c>
       <c r="AB62">
         <v>14838</v>
       </c>
@@ -2377,6 +2537,10 @@
         <f>N59+N60+N61+N62</f>
         <v>125115</v>
       </c>
+      <c r="R63">
+        <f>R59+R60+R61+R62</f>
+        <v>137849</v>
+      </c>
       <c r="AB63">
         <f>AB59+AB60+AB61+AB62</f>
         <v>103498</v>
@@ -2396,6 +2560,9 @@
       <c r="N65">
         <v>1329</v>
       </c>
+      <c r="R65">
+        <v>544</v>
+      </c>
       <c r="AB65">
         <v>1527</v>
       </c>
@@ -2413,6 +2580,9 @@
       <c r="N66">
         <v>207554</v>
       </c>
+      <c r="R66">
+        <v>191712</v>
+      </c>
       <c r="AB66">
         <v>216054</v>
       </c>
@@ -2424,6 +2594,9 @@
       <c r="A67" t="s">
         <v>43</v>
       </c>
+      <c r="R67">
+        <v>81569</v>
+      </c>
       <c r="AC67">
         <v>80202</v>
       </c>
@@ -2438,6 +2611,9 @@
       <c r="N68">
         <v>5137</v>
       </c>
+      <c r="R68">
+        <v>2600</v>
+      </c>
       <c r="AB68">
         <v>5468</v>
       </c>
@@ -2457,6 +2633,10 @@
         <f>N63+N65+N66+N67+N68</f>
         <v>339135</v>
       </c>
+      <c r="R69">
+        <f>R63+R65+R66+R67+R68</f>
+        <v>414274</v>
+      </c>
       <c r="AB69">
         <f>AB63+AB65+AB66+AB67+AB68</f>
         <v>326547</v>
@@ -2478,6 +2658,9 @@
       <c r="N72">
         <v>8523</v>
       </c>
+      <c r="R72">
+        <v>6173</v>
+      </c>
       <c r="AB72">
         <v>6685</v>
       </c>
@@ -2492,6 +2675,9 @@
       <c r="N73">
         <v>55588</v>
       </c>
+      <c r="R73">
+        <v>52313</v>
+      </c>
       <c r="AB73">
         <v>52662</v>
       </c>
@@ -2506,6 +2692,9 @@
       <c r="N74">
         <v>15386</v>
       </c>
+      <c r="R74">
+        <v>10799</v>
+      </c>
       <c r="AB74">
         <v>14699</v>
       </c>
@@ -2520,6 +2709,9 @@
       <c r="N75">
         <v>12271</v>
       </c>
+      <c r="R75">
+        <v>470</v>
+      </c>
       <c r="AB75">
         <v>12174</v>
       </c>
@@ -2534,6 +2726,9 @@
       <c r="N76">
         <v>14600</v>
       </c>
+      <c r="R76">
+        <v>24458</v>
+      </c>
       <c r="AB76">
         <v>14500</v>
       </c>
@@ -2548,6 +2743,9 @@
       <c r="N77">
         <v>32159</v>
       </c>
+      <c r="R77">
+        <v>332</v>
+      </c>
       <c r="AB77">
         <v>34299</v>
       </c>
@@ -2563,6 +2761,10 @@
         <f>N72+N73+N74+N75+N76+N77</f>
         <v>138527</v>
       </c>
+      <c r="R78">
+        <f>R72+R73+R74+R75+R76+R77</f>
+        <v>94545</v>
+      </c>
       <c r="AB78">
         <f>AB72+AB73+AB74+AB75+AB76+AB77</f>
         <v>135019</v>
@@ -2579,6 +2781,9 @@
       <c r="N80">
         <v>61250</v>
       </c>
+      <c r="R80">
+        <v>38151</v>
+      </c>
       <c r="AB80">
         <v>61319</v>
       </c>
@@ -2593,6 +2798,9 @@
       <c r="N81">
         <v>22859</v>
       </c>
+      <c r="R81">
+        <v>26600</v>
+      </c>
       <c r="AB81">
         <v>23159</v>
       </c>
@@ -2607,6 +2815,9 @@
       <c r="N82">
         <v>4637</v>
       </c>
+      <c r="R82">
+        <v>4314</v>
+      </c>
       <c r="AB82">
         <v>4636</v>
       </c>
@@ -2622,6 +2833,10 @@
         <f>N78+N80+N81+N82</f>
         <v>227273</v>
       </c>
+      <c r="R83">
+        <f>R78+R80+R81+R82</f>
+        <v>163610</v>
+      </c>
       <c r="AB83">
         <f>AB78+AB80+AB81+AB82</f>
         <v>224133</v>
@@ -2643,6 +2858,9 @@
       <c r="N86">
         <v>4</v>
       </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
       <c r="AB86">
         <v>4</v>
       </c>
@@ -2654,8 +2872,14 @@
       <c r="A87" t="s">
         <v>135</v>
       </c>
+      <c r="M87">
+        <v>48319838</v>
+      </c>
       <c r="N87">
         <v>45335426</v>
+      </c>
+      <c r="R87">
+        <v>55661866</v>
       </c>
       <c r="AB87">
         <v>44640444</v>
@@ -2671,6 +2895,9 @@
       <c r="N88">
         <v>532020</v>
       </c>
+      <c r="R88">
+        <v>573744</v>
+      </c>
       <c r="AB88">
         <v>531636</v>
       </c>
@@ -2685,6 +2912,9 @@
       <c r="N89">
         <v>-420162</v>
       </c>
+      <c r="R89">
+        <v>-323085</v>
+      </c>
       <c r="AB89">
         <v>-429226</v>
       </c>
@@ -2700,6 +2930,10 @@
         <f>N86+N88+N89</f>
         <v>111862</v>
       </c>
+      <c r="R90">
+        <f>R86+R88+R89</f>
+        <v>250664</v>
+      </c>
       <c r="AB90">
         <f>AB86+AB88+AB89</f>
         <v>102414</v>
@@ -2717,6 +2951,10 @@
         <f>N90+N83</f>
         <v>339135</v>
       </c>
+      <c r="R92">
+        <f>R90+R83</f>
+        <v>414274</v>
+      </c>
       <c r="AB92">
         <f>AB90+AB83</f>
         <v>326547</v>
@@ -2732,6 +2970,10 @@
       </c>
       <c r="N93">
         <f>N92-N69</f>
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <f>R92-R69</f>
         <v>0</v>
       </c>
       <c r="AB93">

</xml_diff>